<commit_message>
Completed code and results from a web scrape
</commit_message>
<xml_diff>
--- a/ASINS_to_scrape.xlsx
+++ b/ASINS_to_scrape.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>ASIN</t>
   </si>
@@ -42,6 +42,21 @@
   </si>
   <si>
     <t>B06XXKQP32</t>
+  </si>
+  <si>
+    <t>abc123xyz</t>
+  </si>
+  <si>
+    <t>B06Y5LXM9T</t>
+  </si>
+  <si>
+    <t>B06WGKYSPD</t>
+  </si>
+  <si>
+    <t>B074F388BG</t>
+  </si>
+  <si>
+    <t>abc123xyz2</t>
   </si>
 </sst>
 </file>
@@ -374,10 +389,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -402,12 +417,37 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added .txt summary file, improved scraper speed because it was slower after each produce code
</commit_message>
<xml_diff>
--- a/ASINS_to_scrape.xlsx
+++ b/ASINS_to_scrape.xlsx
@@ -1,19 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\18047\Documents\Github\Amazon-Scrape\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mark0\Desktop\Amazon-scrape\Amazon-scrape\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4F94325-287E-4204-8266-684A677A8A5C}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10365" windowHeight="4080"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId2"/>
+  </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1</definedName>
   </definedNames>
@@ -27,42 +31,153 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>ASIN</t>
   </si>
   <si>
-    <t>B075KNSDR7</t>
-  </si>
-  <si>
-    <t>B073SCXP26</t>
-  </si>
-  <si>
-    <t>B06XDJP2WX</t>
-  </si>
-  <si>
-    <t>B06XXKQP32</t>
-  </si>
-  <si>
-    <t>abc123xyz</t>
-  </si>
-  <si>
-    <t>B06Y5LXM9T</t>
-  </si>
-  <si>
-    <t>B06WGKYSPD</t>
-  </si>
-  <si>
-    <t>B074F388BG</t>
-  </si>
-  <si>
-    <t>abc123xyz2</t>
+    <t>B00M9M8MFC</t>
+  </si>
+  <si>
+    <t>B07D4NS4CZ</t>
+  </si>
+  <si>
+    <t>B00HT72O2O</t>
+  </si>
+  <si>
+    <t>B003ZJQHSM</t>
+  </si>
+  <si>
+    <t>B07CV54ZCL</t>
+  </si>
+  <si>
+    <t>B003WG54TQ</t>
+  </si>
+  <si>
+    <t>B07CV4L94Y</t>
+  </si>
+  <si>
+    <t>B00M9MGUQ0</t>
+  </si>
+  <si>
+    <t>B07DFMWF37</t>
+  </si>
+  <si>
+    <t>B00OQMVU4S</t>
+  </si>
+  <si>
+    <t>B001J3ZUQ6</t>
+  </si>
+  <si>
+    <t>B00M9NLJWO</t>
+  </si>
+  <si>
+    <t>B00GO6GUIU</t>
+  </si>
+  <si>
+    <t>B00M9NJ5ES</t>
+  </si>
+  <si>
+    <t>B003ZJQBLA</t>
+  </si>
+  <si>
+    <t>B00VJMJZ1I</t>
+  </si>
+  <si>
+    <t>B0140NBD9Y</t>
+  </si>
+  <si>
+    <t>B003ZJJ4K0</t>
+  </si>
+  <si>
+    <t>B003ZJKOZE</t>
+  </si>
+  <si>
+    <t>B003W0JWCC</t>
+  </si>
+  <si>
+    <t>B00HT84LFQ</t>
+  </si>
+  <si>
+    <t>B00GP0EZ14</t>
+  </si>
+  <si>
+    <t>B00QR6JMH8</t>
+  </si>
+  <si>
+    <t>B00017LEZC</t>
+  </si>
+  <si>
+    <t>B00G5IWQ3U</t>
+  </si>
+  <si>
+    <t>B001J4FSR6</t>
+  </si>
+  <si>
+    <t>B07CV2WJ3L</t>
+  </si>
+  <si>
+    <t>B00M9NO8PO</t>
+  </si>
+  <si>
+    <t>B00M9NG2J4</t>
+  </si>
+  <si>
+    <t>B00INM1OQ6</t>
+  </si>
+  <si>
+    <t>B003ZJKG1G</t>
+  </si>
+  <si>
+    <t>B00M9NDB1Q</t>
+  </si>
+  <si>
+    <t>B00M9NJXJK</t>
+  </si>
+  <si>
+    <t>B00MARRI10</t>
+  </si>
+  <si>
+    <t>B00VDWVM7Y</t>
+  </si>
+  <si>
+    <t>B00M9NI7IS</t>
+  </si>
+  <si>
+    <t>B003W0KBFE</t>
+  </si>
+  <si>
+    <t>B00AX6JGI8</t>
+  </si>
+  <si>
+    <t>B075FD8XLP</t>
+  </si>
+  <si>
+    <t>B00017LEYI</t>
+  </si>
+  <si>
+    <t>B075FDHHVG</t>
+  </si>
+  <si>
+    <t>B003WGE3ES</t>
+  </si>
+  <si>
+    <t>B00NJ1NX7E</t>
+  </si>
+  <si>
+    <t>B07CV4B86R</t>
+  </si>
+  <si>
+    <t>B00UHKJG8A</t>
+  </si>
+  <si>
+    <t>B00HW2IFPG</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -106,14 +221,30 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFDEED7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFAD194"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -124,6 +255,23 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Sheet 1"/>
+      <sheetName val="Sheet 2"/>
+      <sheetName val="Sheet 3"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -388,11 +536,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:A47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A2" sqref="A2:A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -406,53 +554,270 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>2</v>
-      </c>
-    </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>7</v>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1"/>
+  <autoFilter ref="A1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="1" id="{EF1258A8-50D8-4ACE-A5A5-92B8722CB9E3}">
+            <xm:f>'\Users\mark0\Desktop\[Amish Country Popcorn - Amish Country Popcorn_ Grocery &amp; Gourmet Food-PC2-20181128.xlsx]Sheet 2'!#REF!="AM"</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFAD194"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>A2:A47</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="2" id="{822A3976-AA55-40B1-82B4-F0271F4855AD}">
+            <xm:f>'\Users\mark0\Desktop\[Amish Country Popcorn - Amish Country Popcorn_ Grocery &amp; Gourmet Food-PC2-20181128.xlsx]Sheet 2'!#REF!="Y"</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFDEED7"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>A2:A47</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>